<commit_message>
update archieve result , log , time cal
</commit_message>
<xml_diff>
--- a/Paper/DQN/Archive_Result/Result_summary.xlsx
+++ b/Paper/DQN/Archive_Result/Result_summary.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="11130" windowHeight="7470" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="21270" windowHeight="5595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>File Name</t>
   </si>
@@ -122,19 +121,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>v6_4_e200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>+100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Processing time</t>
+    <t>v6_4_e100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>~40 hour</t>
+    <t>v6_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v6_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Processing time (hours)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v6_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Activation function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>relu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,25 +475,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.875" customWidth="1"/>
-    <col min="14" max="15" width="21.875" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22" customWidth="1"/>
-    <col min="18" max="18" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.875" customWidth="1"/>
+    <col min="15" max="16" width="21.875" customWidth="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22" customWidth="1"/>
+    <col min="19" max="19" width="25.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,52 +505,55 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
-        <v>34</v>
-      </c>
       <c r="R1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -544,47 +563,50 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
       <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.9</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2000</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>100000</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>50</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>100</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>300</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1000</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.2</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.62260000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -594,47 +616,50 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3">
         <v>240</v>
       </c>
-      <c r="E3">
-        <v>0.1</v>
-      </c>
       <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.9</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>500</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5000</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>50</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>100</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>300</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1000</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>2000</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>1.1047</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -644,47 +669,50 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4">
         <v>240</v>
       </c>
-      <c r="E4">
-        <v>0.1</v>
-      </c>
       <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.9</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>150</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5000</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
       </c>
       <c r="K4">
         <v>100</v>
       </c>
       <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4">
         <v>300</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>5000</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.2</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>2.3896999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -694,47 +722,50 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5">
         <v>30</v>
       </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
       <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.9</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2000</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>10000</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>50</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>100</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>300</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>2000</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>4000</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.2</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.11466</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -744,47 +775,50 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6">
         <v>240</v>
       </c>
-      <c r="E6">
-        <v>0.1</v>
-      </c>
       <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>150</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>100000</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
       </c>
       <c r="K6">
         <v>100</v>
       </c>
       <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
         <v>300</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>5000</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.2</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>3.5651999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -794,47 +828,50 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
         <v>240</v>
       </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
       <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>150</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>100000</v>
-      </c>
-      <c r="J7">
-        <v>100</v>
       </c>
       <c r="K7">
         <v>100</v>
       </c>
       <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7">
         <v>300</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>5000</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.2</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>3.4304000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -844,44 +881,47 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
         <v>240</v>
       </c>
-      <c r="E8">
-        <v>0.1</v>
-      </c>
       <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.95</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>150</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>100000</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>100</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>200</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>300</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>0</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>5000</v>
       </c>
-      <c r="O8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="P8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -891,50 +931,53 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9">
         <v>240</v>
       </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
       <c r="F9">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.95</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>150</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>100000</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>100</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>200</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>300</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>5000</v>
       </c>
-      <c r="O9">
-        <v>0.1</v>
-      </c>
       <c r="P9">
+        <v>0.1</v>
+      </c>
+      <c r="Q9">
         <v>0.82099999999999995</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -944,47 +987,50 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10">
         <v>240</v>
       </c>
-      <c r="E10">
-        <v>0.1</v>
-      </c>
       <c r="F10">
+        <v>0.1</v>
+      </c>
+      <c r="G10">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.95</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>150</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>100000</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>100</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>200</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>300</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>0</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>1000</v>
       </c>
-      <c r="O10">
-        <v>0.1</v>
-      </c>
       <c r="P10">
+        <v>0.1</v>
+      </c>
+      <c r="Q10">
         <v>1.4375</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -994,50 +1040,53 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
         <v>240</v>
       </c>
-      <c r="E11">
-        <v>0.1</v>
-      </c>
       <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>300</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>1000000</v>
-      </c>
-      <c r="J11">
-        <v>200</v>
       </c>
       <c r="K11">
         <v>200</v>
       </c>
       <c r="L11">
+        <v>200</v>
+      </c>
+      <c r="M11">
         <v>600</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>0</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>10000</v>
       </c>
-      <c r="O11">
-        <v>0.1</v>
-      </c>
       <c r="P11">
+        <v>0.1</v>
+      </c>
+      <c r="Q11">
         <v>3.5920999999999998</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1047,97 +1096,215 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12">
         <v>240</v>
       </c>
-      <c r="E12">
-        <v>0.1</v>
-      </c>
       <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>100</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1000000</v>
-      </c>
-      <c r="J12">
-        <v>200</v>
       </c>
       <c r="K12">
         <v>200</v>
       </c>
       <c r="L12">
+        <v>200</v>
+      </c>
+      <c r="M12">
         <v>600</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>0</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>10000</v>
       </c>
-      <c r="O12">
-        <v>0.1</v>
-      </c>
       <c r="P12">
+        <v>0.1</v>
+      </c>
+      <c r="Q12">
         <v>1.8259000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13">
         <v>240</v>
       </c>
-      <c r="E13">
-        <v>0.1</v>
-      </c>
       <c r="F13">
+        <v>0.1</v>
+      </c>
+      <c r="G13">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>9.0000000000000002E-6</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13">
+      <c r="I13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13">
         <v>1000000</v>
-      </c>
-      <c r="J13">
-        <v>200</v>
       </c>
       <c r="K13">
         <v>200</v>
       </c>
       <c r="L13">
+        <v>200</v>
+      </c>
+      <c r="M13">
         <v>600</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>0</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>10000</v>
       </c>
-      <c r="O13">
-        <v>0.1</v>
-      </c>
       <c r="P13">
+        <v>0.1</v>
+      </c>
+      <c r="Q13">
         <v>3.6585999999999999</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
         <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14">
+        <v>240</v>
+      </c>
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+      <c r="G14">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H14">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="I14">
+        <v>1660</v>
+      </c>
+      <c r="J14">
+        <v>1000000</v>
+      </c>
+      <c r="K14">
+        <v>50</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <v>600</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>1000</v>
+      </c>
+      <c r="P14">
+        <v>0.1</v>
+      </c>
+      <c r="Q14">
+        <v>2.7909000000000002</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <v>240</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H15">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="I15">
+        <v>2000</v>
+      </c>
+      <c r="J15">
+        <v>1000000</v>
+      </c>
+      <c r="K15">
+        <v>50</v>
+      </c>
+      <c r="L15">
+        <v>300</v>
+      </c>
+      <c r="M15">
+        <v>600</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1000</v>
+      </c>
+      <c r="P15">
+        <v>0.1</v>
+      </c>
+      <c r="Q15">
+        <v>2.9058999999999999</v>
+      </c>
+      <c r="R15">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>